<commit_message>
Reviewed & fixed up 2018 & 2020 data
</commit_message>
<xml_diff>
--- a/data/extracted/Congressional Election Results by State (2000 - 107th).xlsx
+++ b/data/extracted/Congressional Election Results by State (2000 - 107th).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/ushouse/data/extracted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14860F35-63FB-6842-9D18-0A72B7135377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CD5C3E-17CD-F34D-9E5E-8FFBC1696D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="500" windowWidth="23020" windowHeight="15560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="174">
   <si>
     <t>Votes</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t>DISTRICT</t>
+  </si>
+  <si>
+    <t>Fixed total which was causing a negative "other".</t>
   </si>
 </sst>
 </file>
@@ -662,7 +665,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,6 +687,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -803,6 +812,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5451,10 +5461,10 @@
   <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:J1048576"/>
+      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6732,10 +6742,10 @@
       </c>
       <c r="F39" s="13">
         <f t="shared" ref="F39:F40" si="6">G39-SUM(D39:E39)</f>
-        <v>-59486</v>
-      </c>
-      <c r="G39" s="1">
-        <v>83960</v>
+        <v>40514</v>
+      </c>
+      <c r="G39" s="40">
+        <v>183960</v>
       </c>
       <c r="H39" s="14">
         <v>1</v>
@@ -6745,6 +6755,9 @@
       </c>
       <c r="J39">
         <v>0</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -8587,11 +8600,11 @@
       </c>
       <c r="F96" s="17">
         <f t="shared" si="14"/>
-        <v>1343063</v>
+        <v>1443063</v>
       </c>
       <c r="G96" s="17">
         <f t="shared" si="14"/>
-        <v>11297389</v>
+        <v>11397389</v>
       </c>
       <c r="H96" s="19">
         <f t="shared" si="14"/>
@@ -11185,10 +11198,10 @@
   <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A94" sqref="A94:J95"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12394,10 +12407,10 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>-59486</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>83960</v>
+        <v>183960</v>
       </c>
       <c r="H38">
         <v>1</v>

</xml_diff>

<commit_message>
Reviewed 2004 & 2006 extracted data
</commit_message>
<xml_diff>
--- a/data/extracted/Congressional Election Results by State (2000 - 107th).xlsx
+++ b/data/extracted/Congressional Election Results by State (2000 - 107th).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/ushouse/data/extracted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CD5C3E-17CD-F34D-9E5E-8FFBC1696D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BFAC90-0180-DE4B-B5B3-6895CAE2CEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="500" windowWidth="23020" windowHeight="15560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11201,7 +11201,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>